<commit_message>
Updated planning sheet with some status infos.
</commit_message>
<xml_diff>
--- a/01_Planning/InitalPlanning.xlsx
+++ b/01_Planning/InitalPlanning.xlsx
@@ -6,20 +6,36 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Ressource Planning - Ressource " sheetId="1" r:id="rId4"/>
-    <sheet name="Ressource Planning - Prios as N" sheetId="2" r:id="rId5"/>
-    <sheet name="Ressource Planning - Priorities" sheetId="3" r:id="rId6"/>
-    <sheet name="First User Stories" sheetId="4" r:id="rId7"/>
+    <sheet name="Export Summary" sheetId="1" r:id="rId4"/>
+    <sheet name="Ressource Planning - Ressource " sheetId="2" r:id="rId5"/>
+    <sheet name="Ressource Planning - Prios as N" sheetId="3" r:id="rId6"/>
+    <sheet name="Ressource Planning - Priorities" sheetId="4" r:id="rId7"/>
+    <sheet name="First User Stories" sheetId="5" r:id="rId8"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="78">
+  <si>
+    <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
+  </si>
+  <si>
+    <t>Numbers Sheet Name</t>
+  </si>
+  <si>
+    <t>Numbers Table Name</t>
+  </si>
+  <si>
+    <t>Excel Worksheet Name</t>
+  </si>
   <si>
     <t>Ressource Planning</t>
   </si>
   <si>
+    <t xml:space="preserve">Ressource Planning - Ressource </t>
+  </si>
+  <si>
     <t>Topic</t>
   </si>
   <si>
@@ -33,6 +49,9 @@
   </si>
   <si>
     <t>Remarks</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
   <si>
     <t>Exchange Sue</t>
@@ -54,9 +73,15 @@
     <t>Ball</t>
   </si>
   <si>
+    <t>Jul06: Sent e-mail and asked for price and shipping costs.</t>
+  </si>
+  <si>
     <t>Own lockable room</t>
   </si>
   <si>
+    <t>Jul06: Clarified with Mr. Mörixbauer and Mr. Holzer that we can use a part of the room opposite to the music room (where the desks are currently stored). Room will be available by start of next school year.</t>
+  </si>
+  <si>
     <t>Bitbucket repository</t>
   </si>
   <si>
@@ -64,6 +89,33 @@
   </si>
   <si>
     <t>Bauepete</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">Jul05: Bitbucket not feasible since max 5 team members are allowed. Repository at </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>gitlab.htl-leonding.ac.at</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> now set up. All team members have accounts and are member of the gitlab group. DONE.</t>
+    </r>
   </si>
   <si>
     <t>Check SPL Site regularly</t>
@@ -202,12 +254,18 @@
     <t>Prios as Numbers</t>
   </si>
   <si>
+    <t>Ressource Planning - Prios as N</t>
+  </si>
+  <si>
     <t>Prio</t>
   </si>
   <si>
     <t>Priorities</t>
   </si>
   <si>
+    <t>Ressource Planning - Priorities</t>
+  </si>
+  <si>
     <t>July 5 onwards</t>
   </si>
   <si>
@@ -218,6 +276,12 @@
   </si>
   <si>
     <t>From December onwards</t>
+  </si>
+  <si>
+    <t>First User Stories</t>
+  </si>
+  <si>
+    <t>Table 1</t>
   </si>
   <si>
     <t>Id</t>
@@ -245,7 +309,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -254,6 +318,17 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="12"/>
+      <color indexed="11"/>
       <name val="Helvetica"/>
     </font>
     <font>
@@ -269,7 +344,7 @@
       <name val="Helvetica"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,7 +359,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="12"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -299,106 +386,106 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -408,20 +495,27 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -433,7 +527,7 @@
     <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -460,16 +554,16 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -478,10 +572,10 @@
     <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -504,6 +598,9 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="015e88b1"/>
+      <rgbColor rgb="01eef3f4"/>
+      <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
@@ -1598,539 +1695,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A2:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="34.9453" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.67188" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.17188" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="26.8047" style="1" customWidth="1"/>
-    <col min="6" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="4" width="33.6016" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="28" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="3" ht="50" customHeight="1">
+      <c r="B3" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="C3"/>
+      <c r="D3"/>
+    </row>
+    <row r="7">
+      <c r="B7" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="C7" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="D7" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="3">
+    </row>
+    <row r="9">
+      <c r="B9" t="s" s="3">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="4"/>
+      <c r="C10" t="s" s="4">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="3" ht="20.55" customHeight="1">
-      <c r="A3" t="s" s="4">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s" s="5">
-        <v>7</v>
-      </c>
-      <c r="C3" s="6">
-        <f>VLOOKUP(B3,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>1</v>
-      </c>
-      <c r="D3" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="E3" s="7"/>
-    </row>
-    <row r="4" ht="32.35" customHeight="1">
-      <c r="A4" t="s" s="8">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s" s="9">
-        <v>7</v>
-      </c>
-      <c r="C4" s="10">
-        <f>VLOOKUP(B4,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>1</v>
-      </c>
-      <c r="D4" t="s" s="11">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s" s="11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" t="s" s="8">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s" s="9">
-        <v>7</v>
-      </c>
-      <c r="C5" s="10">
-        <f>VLOOKUP(B5,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>1</v>
-      </c>
-      <c r="D5" t="s" s="11">
-        <v>8</v>
-      </c>
-      <c r="E5" s="11"/>
-    </row>
-    <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" t="s" s="8">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s" s="9">
-        <v>7</v>
-      </c>
-      <c r="C6" s="10">
-        <f>VLOOKUP(B6,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>1</v>
-      </c>
-      <c r="D6" t="s" s="11">
-        <v>8</v>
-      </c>
-      <c r="E6" s="11"/>
-    </row>
-    <row r="7" ht="20.35" customHeight="1">
-      <c r="A7" t="s" s="8">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s" s="9">
-        <v>7</v>
-      </c>
-      <c r="C7" s="10">
-        <f>VLOOKUP(B7,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>1</v>
-      </c>
-      <c r="D7" t="s" s="11">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s" s="11">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" ht="32.35" customHeight="1">
-      <c r="A8" t="s" s="8">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s" s="9">
-        <v>7</v>
-      </c>
-      <c r="C8" s="10">
-        <f>VLOOKUP(B8,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>1</v>
-      </c>
-      <c r="D8" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s" s="11">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s" s="9">
-        <v>7</v>
-      </c>
-      <c r="C9" s="10">
-        <f>VLOOKUP(B9,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>1</v>
-      </c>
-      <c r="D9" t="s" s="11">
-        <v>14</v>
-      </c>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" t="s" s="8">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s" s="9">
-        <v>7</v>
-      </c>
-      <c r="C10" s="10">
-        <f>VLOOKUP(B10,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>1</v>
-      </c>
-      <c r="D10" t="s" s="11">
-        <v>8</v>
-      </c>
-      <c r="E10" s="11"/>
-    </row>
-    <row r="11" ht="20.35" customHeight="1">
-      <c r="A11" t="s" s="8">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s" s="9">
-        <v>22</v>
-      </c>
-      <c r="C11" s="10">
-        <f>VLOOKUP(B11,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>2</v>
-      </c>
-      <c r="D11" t="s" s="11">
-        <v>8</v>
-      </c>
-      <c r="E11" s="12"/>
-    </row>
-    <row r="12" ht="20.35" customHeight="1">
-      <c r="A12" t="s" s="8">
-        <v>23</v>
-      </c>
-      <c r="B12" t="s" s="9">
-        <v>22</v>
-      </c>
-      <c r="C12" s="10">
-        <f>VLOOKUP(B12,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>2</v>
-      </c>
-      <c r="D12" t="s" s="11">
-        <v>8</v>
-      </c>
-      <c r="E12" s="12"/>
-    </row>
-    <row r="13" ht="20.35" customHeight="1">
-      <c r="A13" t="s" s="8">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s" s="9">
-        <v>22</v>
-      </c>
-      <c r="C13" s="10">
-        <f>VLOOKUP(B13,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>2</v>
-      </c>
-      <c r="D13" t="s" s="11">
-        <v>25</v>
-      </c>
-      <c r="E13" s="12"/>
-    </row>
-    <row r="14" ht="20.35" customHeight="1">
-      <c r="A14" t="s" s="8">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s" s="9">
-        <v>22</v>
-      </c>
-      <c r="C14" s="10">
-        <f>VLOOKUP(B14,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>2</v>
-      </c>
-      <c r="D14" t="s" s="11">
-        <v>14</v>
-      </c>
-      <c r="E14" s="12"/>
-    </row>
-    <row r="15" ht="20.35" customHeight="1">
-      <c r="A15" t="s" s="8">
-        <v>27</v>
-      </c>
-      <c r="B15" t="s" s="9">
-        <v>22</v>
-      </c>
-      <c r="C15" s="10">
-        <f>VLOOKUP(B15,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>2</v>
-      </c>
-      <c r="D15" t="s" s="11">
-        <v>8</v>
-      </c>
-      <c r="E15" s="12"/>
-    </row>
-    <row r="16" ht="20.35" customHeight="1">
-      <c r="A16" t="s" s="8">
-        <v>28</v>
-      </c>
-      <c r="B16" t="s" s="9">
-        <v>22</v>
-      </c>
-      <c r="C16" s="10">
-        <f>VLOOKUP(B16,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>2</v>
-      </c>
-      <c r="D16" t="s" s="11">
-        <v>25</v>
-      </c>
-      <c r="E16" t="s" s="11">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" ht="20.35" customHeight="1">
-      <c r="A17" t="s" s="8">
-        <v>30</v>
-      </c>
-      <c r="B17" t="s" s="9">
-        <v>22</v>
-      </c>
-      <c r="C17" s="10">
-        <f>VLOOKUP(B17,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>2</v>
-      </c>
-      <c r="D17" t="s" s="11">
-        <v>14</v>
-      </c>
-      <c r="E17" t="s" s="11">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" ht="20.35" customHeight="1">
-      <c r="A18" t="s" s="8">
-        <v>32</v>
-      </c>
-      <c r="B18" t="s" s="9">
-        <v>22</v>
-      </c>
-      <c r="C18" s="10">
-        <f>VLOOKUP(B18,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>2</v>
-      </c>
-      <c r="D18" t="s" s="11">
-        <v>8</v>
-      </c>
-      <c r="E18" s="12"/>
-    </row>
-    <row r="19" ht="20.35" customHeight="1">
-      <c r="A19" t="s" s="8">
-        <v>33</v>
-      </c>
-      <c r="B19" t="s" s="9">
-        <v>22</v>
-      </c>
-      <c r="C19" s="10">
-        <f>VLOOKUP(B19,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>2</v>
-      </c>
-      <c r="D19" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="E19" t="s" s="11">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" ht="20.35" customHeight="1">
-      <c r="A20" t="s" s="8">
-        <v>35</v>
-      </c>
-      <c r="B20" t="s" s="9">
-        <v>36</v>
-      </c>
-      <c r="C20" s="10">
-        <f>VLOOKUP(B20,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>3</v>
-      </c>
-      <c r="D20" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="E20" s="11"/>
-    </row>
-    <row r="21" ht="20.35" customHeight="1">
-      <c r="A21" t="s" s="8">
-        <v>37</v>
-      </c>
-      <c r="B21" t="s" s="9">
-        <v>36</v>
-      </c>
-      <c r="C21" s="10">
-        <f>VLOOKUP(B21,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>3</v>
-      </c>
-      <c r="D21" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="E21" s="11"/>
-    </row>
-    <row r="22" ht="32.35" customHeight="1">
-      <c r="A22" t="s" s="8">
-        <v>38</v>
-      </c>
-      <c r="B22" t="s" s="9">
-        <v>36</v>
-      </c>
-      <c r="C22" s="10">
-        <f>VLOOKUP(B22,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>3</v>
-      </c>
-      <c r="D22" t="s" s="11">
-        <v>25</v>
-      </c>
-      <c r="E22" t="s" s="11">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" ht="32.35" customHeight="1">
-      <c r="A23" t="s" s="8">
-        <v>40</v>
-      </c>
-      <c r="B23" t="s" s="9">
-        <v>36</v>
-      </c>
-      <c r="C23" s="10">
-        <f>VLOOKUP(B23,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>3</v>
-      </c>
-      <c r="D23" t="s" s="11">
-        <v>8</v>
-      </c>
-      <c r="E23" s="11"/>
-    </row>
-    <row r="24" ht="20.35" customHeight="1">
-      <c r="A24" t="s" s="8">
-        <v>41</v>
-      </c>
-      <c r="B24" t="s" s="9">
-        <v>36</v>
-      </c>
-      <c r="C24" s="10">
-        <f>VLOOKUP(B24,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>3</v>
-      </c>
-      <c r="D24" t="s" s="11">
-        <v>8</v>
-      </c>
-      <c r="E24" s="11"/>
-    </row>
-    <row r="25" ht="20.35" customHeight="1">
-      <c r="A25" t="s" s="8">
-        <v>42</v>
-      </c>
-      <c r="B25" t="s" s="9">
-        <v>43</v>
-      </c>
-      <c r="C25" s="10">
-        <f>VLOOKUP(B25,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>4</v>
-      </c>
-      <c r="D25" t="s" s="11">
-        <v>8</v>
-      </c>
-      <c r="E25" s="11"/>
-    </row>
-    <row r="26" ht="20.35" customHeight="1">
-      <c r="A26" t="s" s="8">
-        <v>44</v>
-      </c>
-      <c r="B26" t="s" s="9">
-        <v>43</v>
-      </c>
-      <c r="C26" s="10">
-        <f>VLOOKUP(B26,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>4</v>
-      </c>
-      <c r="D26" t="s" s="11">
-        <v>8</v>
-      </c>
-      <c r="E26" t="s" s="11">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" ht="20.35" customHeight="1">
-      <c r="A27" t="s" s="8">
-        <v>46</v>
-      </c>
-      <c r="B27" t="s" s="9">
-        <v>43</v>
-      </c>
-      <c r="C27" s="10">
-        <f>VLOOKUP(B27,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>4</v>
-      </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-    </row>
-    <row r="28" ht="20.35" customHeight="1">
-      <c r="A28" t="s" s="8">
-        <v>47</v>
-      </c>
-      <c r="B28" t="s" s="9">
-        <v>43</v>
-      </c>
-      <c r="C28" s="10">
-        <f>VLOOKUP(B28,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>4</v>
-      </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-    </row>
-    <row r="29" ht="20.35" customHeight="1">
-      <c r="A29" t="s" s="8">
-        <v>48</v>
-      </c>
-      <c r="B29" t="s" s="9">
-        <v>43</v>
-      </c>
-      <c r="C29" s="10">
-        <f>VLOOKUP(B29,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>4</v>
-      </c>
-      <c r="D29" t="s" s="11">
-        <v>8</v>
-      </c>
-      <c r="E29" s="11"/>
-    </row>
-    <row r="30" ht="20.35" customHeight="1">
-      <c r="A30" t="s" s="8">
-        <v>49</v>
-      </c>
-      <c r="B30" t="s" s="9">
-        <v>43</v>
-      </c>
-      <c r="C30" s="10">
-        <f>VLOOKUP(B30,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>4</v>
-      </c>
-      <c r="D30" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="E30" s="11"/>
-    </row>
-    <row r="31" ht="20.35" customHeight="1">
-      <c r="A31" t="s" s="8">
-        <v>50</v>
-      </c>
-      <c r="B31" t="s" s="9">
-        <v>43</v>
-      </c>
-      <c r="C31" s="10">
-        <f>VLOOKUP(B31,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
-        <v>4</v>
-      </c>
-      <c r="D31" s="11"/>
-      <c r="E31" t="s" s="11">
-        <v>51</v>
+    <row r="11">
+      <c r="B11" s="4"/>
+      <c r="C11" t="s" s="4">
+        <v>61</v>
+      </c>
+      <c r="D11" t="s" s="5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="4"/>
+      <c r="C12" t="s" s="4">
+        <v>64</v>
+      </c>
+      <c r="D12" t="s" s="5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s" s="3">
+        <v>70</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14">
+      <c r="B14" s="4"/>
+      <c r="C14" t="s" s="4">
+        <v>71</v>
+      </c>
+      <c r="D14" t="s" s="5">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E22" r:id="rId1" location="" tooltip="" display=""/>
+    <hyperlink ref="D10" location="'Ressource Planning - Ressource '!R2C1" tooltip="" display="Ressource Planning - Ressource "/>
+    <hyperlink ref="D11" location="'Ressource Planning - Prios as N'!R2C1" tooltip="" display="Ressource Planning - Prios as N"/>
+    <hyperlink ref="D12" location="'Ressource Planning - Priorities'!R2C1" tooltip="" display="Ressource Planning - Priorities"/>
+    <hyperlink ref="D14" location="'First User Stories'!R1C1" tooltip="" display="First User Stories"/>
   </hyperlinks>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
 
@@ -2139,7 +1790,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:B6"/>
+  <dimension ref="A2:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -2147,61 +1798,564 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.3516" style="13" customWidth="1"/>
-    <col min="2" max="2" width="16.3516" style="13" customWidth="1"/>
-    <col min="3" max="256" width="16.3516" style="13" customWidth="1"/>
+    <col min="1" max="1" width="34.9453" style="6" customWidth="1"/>
+    <col min="2" max="2" width="8.67188" style="6" customWidth="1"/>
+    <col min="3" max="3" width="6.17188" style="6" customWidth="1"/>
+    <col min="4" max="4" width="11.3516" style="6" customWidth="1"/>
+    <col min="5" max="5" width="26.8047" style="6" customWidth="1"/>
+    <col min="6" max="6" width="26.8047" style="6" customWidth="1"/>
+    <col min="7" max="256" width="16.3516" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="28" customHeight="1">
-      <c r="A1" t="s" s="2">
+      <c r="A1" t="s" s="7">
+        <v>4</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" ht="20.55" customHeight="1">
+      <c r="A2" t="s" s="8">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s" s="8">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s" s="8">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s" s="8">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s" s="8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" ht="20.55" customHeight="1">
+      <c r="A3" t="s" s="9">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s" s="10">
+        <v>13</v>
+      </c>
+      <c r="C3" s="11">
+        <f>VLOOKUP(B3,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>1</v>
+      </c>
+      <c r="D3" t="s" s="12">
+        <v>14</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+    </row>
+    <row r="4" ht="32.35" customHeight="1">
+      <c r="A4" t="s" s="13">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s" s="14">
+        <v>13</v>
+      </c>
+      <c r="C4" s="15">
+        <f>VLOOKUP(B4,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>1</v>
+      </c>
+      <c r="D4" t="s" s="16">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s" s="16">
+        <v>16</v>
+      </c>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" ht="32.35" customHeight="1">
+      <c r="A5" t="s" s="13">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s" s="14">
+        <v>13</v>
+      </c>
+      <c r="C5" s="15">
+        <f>VLOOKUP(B5,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>1</v>
+      </c>
+      <c r="D5" t="s" s="16">
+        <v>14</v>
+      </c>
+      <c r="E5" s="16"/>
+      <c r="F5" t="s" s="16">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" ht="92.35" customHeight="1">
+      <c r="A6" t="s" s="13">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s" s="14">
+        <v>13</v>
+      </c>
+      <c r="C6" s="15">
+        <f>VLOOKUP(B6,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>1</v>
+      </c>
+      <c r="D6" t="s" s="16">
+        <v>14</v>
+      </c>
+      <c r="E6" s="16"/>
+      <c r="F6" t="s" s="16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" ht="92.35" customHeight="1">
+      <c r="A7" t="s" s="13">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s" s="14">
+        <v>13</v>
+      </c>
+      <c r="C7" s="15">
+        <f>VLOOKUP(B7,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>1</v>
+      </c>
+      <c r="D7" t="s" s="16">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s" s="16">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s" s="16">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" ht="32.35" customHeight="1">
+      <c r="A8" t="s" s="13">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s" s="14">
+        <v>13</v>
+      </c>
+      <c r="C8" s="15">
+        <f>VLOOKUP(B8,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>1</v>
+      </c>
+      <c r="D8" t="s" s="16">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s" s="16">
+        <v>27</v>
+      </c>
+      <c r="F8" s="16"/>
+    </row>
+    <row r="9" ht="20.35" customHeight="1">
+      <c r="A9" t="s" s="13">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s" s="14">
+        <v>13</v>
+      </c>
+      <c r="C9" s="15">
+        <f>VLOOKUP(B9,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>1</v>
+      </c>
+      <c r="D9" t="s" s="16">
+        <v>22</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+    </row>
+    <row r="10" ht="20.35" customHeight="1">
+      <c r="A10" t="s" s="13">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s" s="14">
+        <v>13</v>
+      </c>
+      <c r="C10" s="15">
+        <f>VLOOKUP(B10,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>1</v>
+      </c>
+      <c r="D10" t="s" s="16">
+        <v>14</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+    </row>
+    <row r="11" ht="20.35" customHeight="1">
+      <c r="A11" t="s" s="13">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s" s="14">
+        <v>31</v>
+      </c>
+      <c r="C11" s="15">
+        <f>VLOOKUP(B11,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>2</v>
+      </c>
+      <c r="D11" t="s" s="16">
+        <v>14</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+    </row>
+    <row r="12" ht="20.35" customHeight="1">
+      <c r="A12" t="s" s="13">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s" s="14">
+        <v>31</v>
+      </c>
+      <c r="C12" s="15">
+        <f>VLOOKUP(B12,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>2</v>
+      </c>
+      <c r="D12" t="s" s="16">
+        <v>14</v>
+      </c>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+    </row>
+    <row r="13" ht="20.35" customHeight="1">
+      <c r="A13" t="s" s="13">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s" s="14">
+        <v>31</v>
+      </c>
+      <c r="C13" s="15">
+        <f>VLOOKUP(B13,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>2</v>
+      </c>
+      <c r="D13" t="s" s="16">
+        <v>34</v>
+      </c>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+    </row>
+    <row r="14" ht="20.35" customHeight="1">
+      <c r="A14" t="s" s="13">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s" s="14">
+        <v>31</v>
+      </c>
+      <c r="C14" s="15">
+        <f>VLOOKUP(B14,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>2</v>
+      </c>
+      <c r="D14" t="s" s="16">
+        <v>22</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+    </row>
+    <row r="15" ht="20.35" customHeight="1">
+      <c r="A15" t="s" s="13">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s" s="14">
+        <v>31</v>
+      </c>
+      <c r="C15" s="15">
+        <f>VLOOKUP(B15,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>2</v>
+      </c>
+      <c r="D15" t="s" s="16">
+        <v>14</v>
+      </c>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+    </row>
+    <row r="16" ht="20.35" customHeight="1">
+      <c r="A16" t="s" s="13">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s" s="14">
+        <v>31</v>
+      </c>
+      <c r="C16" s="15">
+        <f>VLOOKUP(B16,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>2</v>
+      </c>
+      <c r="D16" t="s" s="16">
+        <v>34</v>
+      </c>
+      <c r="E16" t="s" s="16">
+        <v>38</v>
+      </c>
+      <c r="F16" s="16"/>
+    </row>
+    <row r="17" ht="20.35" customHeight="1">
+      <c r="A17" t="s" s="13">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s" s="14">
+        <v>31</v>
+      </c>
+      <c r="C17" s="15">
+        <f>VLOOKUP(B17,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>2</v>
+      </c>
+      <c r="D17" t="s" s="16">
+        <v>22</v>
+      </c>
+      <c r="E17" t="s" s="16">
+        <v>40</v>
+      </c>
+      <c r="F17" s="16"/>
+    </row>
+    <row r="18" ht="20.35" customHeight="1">
+      <c r="A18" t="s" s="13">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s" s="14">
+        <v>31</v>
+      </c>
+      <c r="C18" s="15">
+        <f>VLOOKUP(B18,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>2</v>
+      </c>
+      <c r="D18" t="s" s="16">
+        <v>14</v>
+      </c>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+    </row>
+    <row r="19" ht="20.35" customHeight="1">
+      <c r="A19" t="s" s="13">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s" s="14">
+        <v>31</v>
+      </c>
+      <c r="C19" s="15">
+        <f>VLOOKUP(B19,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>2</v>
+      </c>
+      <c r="D19" t="s" s="16">
+        <v>26</v>
+      </c>
+      <c r="E19" t="s" s="16">
+        <v>43</v>
+      </c>
+      <c r="F19" s="16"/>
+    </row>
+    <row r="20" ht="20.35" customHeight="1">
+      <c r="A20" t="s" s="13">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s" s="14">
+        <v>45</v>
+      </c>
+      <c r="C20" s="15">
+        <f>VLOOKUP(B20,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>3</v>
+      </c>
+      <c r="D20" t="s" s="16">
+        <v>26</v>
+      </c>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+    </row>
+    <row r="21" ht="20.35" customHeight="1">
+      <c r="A21" t="s" s="13">
+        <v>46</v>
+      </c>
+      <c r="B21" t="s" s="14">
+        <v>45</v>
+      </c>
+      <c r="C21" s="15">
+        <f>VLOOKUP(B21,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>3</v>
+      </c>
+      <c r="D21" t="s" s="16">
+        <v>26</v>
+      </c>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+    </row>
+    <row r="22" ht="32.35" customHeight="1">
+      <c r="A22" t="s" s="13">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s" s="14">
+        <v>45</v>
+      </c>
+      <c r="C22" s="15">
+        <f>VLOOKUP(B22,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>3</v>
+      </c>
+      <c r="D22" t="s" s="16">
+        <v>34</v>
+      </c>
+      <c r="E22" t="s" s="16">
+        <v>48</v>
+      </c>
+      <c r="F22" s="16"/>
+    </row>
+    <row r="23" ht="32.35" customHeight="1">
+      <c r="A23" t="s" s="13">
+        <v>49</v>
+      </c>
+      <c r="B23" t="s" s="14">
+        <v>45</v>
+      </c>
+      <c r="C23" s="15">
+        <f>VLOOKUP(B23,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>3</v>
+      </c>
+      <c r="D23" t="s" s="16">
+        <v>14</v>
+      </c>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+    </row>
+    <row r="24" ht="20.35" customHeight="1">
+      <c r="A24" t="s" s="13">
+        <v>50</v>
+      </c>
+      <c r="B24" t="s" s="14">
+        <v>45</v>
+      </c>
+      <c r="C24" s="15">
+        <f>VLOOKUP(B24,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>3</v>
+      </c>
+      <c r="D24" t="s" s="16">
+        <v>14</v>
+      </c>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+    </row>
+    <row r="25" ht="20.35" customHeight="1">
+      <c r="A25" t="s" s="13">
+        <v>51</v>
+      </c>
+      <c r="B25" t="s" s="14">
         <v>52</v>
       </c>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="C25" s="15">
+        <f>VLOOKUP(B25,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>4</v>
+      </c>
+      <c r="D25" t="s" s="16">
+        <v>14</v>
+      </c>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+    </row>
+    <row r="26" ht="20.35" customHeight="1">
+      <c r="A26" t="s" s="13">
         <v>53</v>
       </c>
-      <c r="B2" t="s" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" ht="20.55" customHeight="1">
-      <c r="A3" t="s" s="4">
-        <v>7</v>
-      </c>
-      <c r="B3" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" t="s" s="8">
-        <v>22</v>
-      </c>
-      <c r="B4" s="15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" t="s" s="8">
-        <v>36</v>
-      </c>
-      <c r="B5" s="15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" t="s" s="8">
-        <v>43</v>
-      </c>
-      <c r="B6" s="15">
+      <c r="B26" t="s" s="14">
+        <v>52</v>
+      </c>
+      <c r="C26" s="15">
+        <f>VLOOKUP(B26,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
         <v>4</v>
       </c>
+      <c r="D26" t="s" s="16">
+        <v>14</v>
+      </c>
+      <c r="E26" t="s" s="16">
+        <v>54</v>
+      </c>
+      <c r="F26" s="16"/>
+    </row>
+    <row r="27" ht="20.35" customHeight="1">
+      <c r="A27" t="s" s="13">
+        <v>55</v>
+      </c>
+      <c r="B27" t="s" s="14">
+        <v>52</v>
+      </c>
+      <c r="C27" s="15">
+        <f>VLOOKUP(B27,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>4</v>
+      </c>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+    </row>
+    <row r="28" ht="20.35" customHeight="1">
+      <c r="A28" t="s" s="13">
+        <v>56</v>
+      </c>
+      <c r="B28" t="s" s="14">
+        <v>52</v>
+      </c>
+      <c r="C28" s="15">
+        <f>VLOOKUP(B28,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>4</v>
+      </c>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+    </row>
+    <row r="29" ht="20.35" customHeight="1">
+      <c r="A29" t="s" s="13">
+        <v>57</v>
+      </c>
+      <c r="B29" t="s" s="14">
+        <v>52</v>
+      </c>
+      <c r="C29" s="15">
+        <f>VLOOKUP(B29,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>4</v>
+      </c>
+      <c r="D29" t="s" s="16">
+        <v>14</v>
+      </c>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+    </row>
+    <row r="30" ht="20.35" customHeight="1">
+      <c r="A30" t="s" s="13">
+        <v>58</v>
+      </c>
+      <c r="B30" t="s" s="14">
+        <v>52</v>
+      </c>
+      <c r="C30" s="15">
+        <f>VLOOKUP(B30,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>4</v>
+      </c>
+      <c r="D30" t="s" s="16">
+        <v>26</v>
+      </c>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+    </row>
+    <row r="31" ht="20.35" customHeight="1">
+      <c r="A31" t="s" s="13">
+        <v>59</v>
+      </c>
+      <c r="B31" t="s" s="14">
+        <v>52</v>
+      </c>
+      <c r="C31" s="15">
+        <f>VLOOKUP(B31,'Ressource Planning - Prios as N'!$A$3:$B$6,2)</f>
+        <v>4</v>
+      </c>
+      <c r="D31" s="16"/>
+      <c r="E31" t="s" s="16">
+        <v>60</v>
+      </c>
+      <c r="F31" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F7" r:id="rId1" location="" tooltip="" display=""/>
+    <hyperlink ref="E22" r:id="rId2" location="" tooltip="" display=""/>
+  </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
@@ -2223,51 +2377,55 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.3516" style="16" customWidth="1"/>
-    <col min="2" max="2" width="20.8516" style="16" customWidth="1"/>
-    <col min="3" max="256" width="16.3516" style="16" customWidth="1"/>
+    <col min="1" max="1" width="16.3516" style="18" customWidth="1"/>
+    <col min="2" max="2" width="16.3516" style="18" customWidth="1"/>
+    <col min="3" max="256" width="16.3516" style="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="28" customHeight="1">
-      <c r="A1" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="B1" s="2"/>
+      <c r="A1" t="s" s="7">
+        <v>61</v>
+      </c>
+      <c r="B1" s="7"/>
     </row>
     <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
+      <c r="A2" t="s" s="8">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s" s="8">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" ht="20.55" customHeight="1">
-      <c r="A3" t="s" s="4">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s" s="5">
-        <v>55</v>
+      <c r="A3" t="s" s="9">
+        <v>13</v>
+      </c>
+      <c r="B3" s="19">
+        <v>1</v>
       </c>
     </row>
     <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" t="s" s="8">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s" s="9">
-        <v>56</v>
+      <c r="A4" t="s" s="13">
+        <v>31</v>
+      </c>
+      <c r="B4" s="20">
+        <v>2</v>
       </c>
     </row>
     <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" t="s" s="8">
-        <v>36</v>
-      </c>
-      <c r="B5" t="s" s="9">
-        <v>57</v>
+      <c r="A5" t="s" s="13">
+        <v>45</v>
+      </c>
+      <c r="B5" s="20">
+        <v>3</v>
       </c>
     </row>
     <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" t="s" s="8">
-        <v>43</v>
-      </c>
-      <c r="B6" t="s" s="9">
-        <v>58</v>
+      <c r="A6" t="s" s="13">
+        <v>52</v>
+      </c>
+      <c r="B6" s="20">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2287,6 +2445,78 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A2:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="16.3516" style="21" customWidth="1"/>
+    <col min="2" max="2" width="20.8516" style="21" customWidth="1"/>
+    <col min="3" max="256" width="16.3516" style="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="28" customHeight="1">
+      <c r="A1" t="s" s="7">
+        <v>64</v>
+      </c>
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" ht="20.55" customHeight="1">
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+    </row>
+    <row r="3" ht="20.55" customHeight="1">
+      <c r="A3" t="s" s="9">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s" s="10">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" ht="20.35" customHeight="1">
+      <c r="A4" t="s" s="13">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s" s="14">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" ht="20.35" customHeight="1">
+      <c r="A5" t="s" s="13">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s" s="14">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" ht="20.35" customHeight="1">
+      <c r="A6" t="s" s="13">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s" s="14">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
@@ -2295,119 +2525,119 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="3" style="18" customWidth="1"/>
-    <col min="2" max="2" width="16.3516" style="18" customWidth="1"/>
-    <col min="3" max="3" width="16.3516" style="18" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="18" customWidth="1"/>
-    <col min="5" max="5" width="16.3516" style="18" customWidth="1"/>
-    <col min="6" max="6" width="16.3516" style="18" customWidth="1"/>
-    <col min="7" max="7" width="16.3516" style="18" customWidth="1"/>
-    <col min="8" max="256" width="16.3516" style="18" customWidth="1"/>
+    <col min="1" max="1" width="3" style="23" customWidth="1"/>
+    <col min="2" max="2" width="16.3516" style="23" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="23" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="23" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="23" customWidth="1"/>
+    <col min="6" max="6" width="16.3516" style="23" customWidth="1"/>
+    <col min="7" max="7" width="16.3516" style="23" customWidth="1"/>
+    <col min="8" max="256" width="16.3516" style="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="32.55" customHeight="1">
-      <c r="A1" t="s" s="3">
-        <v>59</v>
-      </c>
-      <c r="B1" t="s" s="3">
-        <v>60</v>
-      </c>
-      <c r="C1" t="s" s="3">
-        <v>61</v>
-      </c>
-      <c r="D1" t="s" s="3">
-        <v>62</v>
-      </c>
-      <c r="E1" t="s" s="3">
-        <v>63</v>
-      </c>
-      <c r="F1" t="s" s="3">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s" s="3">
-        <v>64</v>
+      <c r="A1" t="s" s="8">
+        <v>72</v>
+      </c>
+      <c r="B1" t="s" s="8">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s" s="8">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s" s="8">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s" s="8">
+        <v>76</v>
+      </c>
+      <c r="F1" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s" s="8">
+        <v>77</v>
       </c>
     </row>
     <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
     </row>
     <row r="3" ht="20.35" customHeight="1">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
     </row>
     <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
     </row>
     <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
     </row>
     <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" s="23"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
     </row>
     <row r="7" ht="20.35" customHeight="1">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" ht="20.35" customHeight="1">
-      <c r="A8" s="23"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
     </row>
     <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
     </row>
     <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>